<commit_message>
Sync data files - 2025-06-30 12:29:26 (       2 files updated)
</commit_message>
<xml_diff>
--- a/Data/Listings/Sidra_listings.xlsx
+++ b/Data/Listings/Sidra_listings.xlsx
@@ -33,7 +33,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -50,11 +50,6 @@
         <fgColor rgb="00FFA500"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ADD8E6"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -69,14 +64,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -636,7 +630,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -745,7 +739,7 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -855,7 +849,7 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -957,7 +951,7 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -1064,7 +1058,7 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -1165,7 +1159,7 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
@@ -1279,7 +1273,7 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -1388,7 +1382,7 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -1493,7 +1487,7 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1588,7 +1582,7 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -1688,7 +1682,7 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -1788,7 +1782,7 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1887,7 +1881,7 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
@@ -1980,7 +1974,7 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
@@ -2070,7 +2064,7 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
@@ -2158,7 +2152,7 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -2275,7 +2269,7 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
@@ -2398,7 +2392,7 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
@@ -2500,7 +2494,7 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
@@ -2604,7 +2598,7 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
@@ -2701,7 +2695,7 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2800,7 +2794,7 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
@@ -2899,7 +2893,7 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
@@ -2994,7 +2988,7 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
@@ -3087,7 +3081,7 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
@@ -3184,7 +3178,7 @@
         </is>
       </c>
       <c r="P27" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
@@ -3300,7 +3294,7 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
@@ -3413,7 +3407,7 @@
         </is>
       </c>
       <c r="P29" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
@@ -3513,7 +3507,7 @@
         </is>
       </c>
       <c r="P30" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
@@ -3614,7 +3608,7 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
@@ -3715,7 +3709,7 @@
         </is>
       </c>
       <c r="P32" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
@@ -3818,7 +3812,7 @@
         </is>
       </c>
       <c r="P33" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
@@ -3918,7 +3912,7 @@
         </is>
       </c>
       <c r="P34" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
@@ -4019,7 +4013,7 @@
         </is>
       </c>
       <c r="P35" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
@@ -4121,7 +4115,7 @@
         </is>
       </c>
       <c r="P36" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
@@ -4223,7 +4217,7 @@
         </is>
       </c>
       <c r="P37" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -4324,7 +4318,7 @@
         </is>
       </c>
       <c r="P38" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
@@ -4405,7 +4399,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -4442,7 +4436,7 @@
         </is>
       </c>
       <c r="P39" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
@@ -4461,7 +4455,7 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>Golden Wave Properties Proudly Presents this amazing E5, 5-bedroom villa located in the heart of Dubai Hills Estate for Sale&lt;br/&gt;&lt;br/&gt;&lt;ul&gt;&lt;li&gt;Spacious 5 bedroom Villa Type E5 for sale in Sidra&lt;/li&gt;&lt;li&gt;Large Corner Plot 6636 sqft in size&lt;/li&gt;&lt;li&gt;BUA 4109.00 SQ FT&lt;/li&gt;&lt;li&gt;Landscaped garden, Well Maintained&lt;/li&gt;&lt;li&gt;Rented for Dhs 560,000/- in ONE PAYMENT till February 2026 and notice has been served for the tenant to vacate at the time of contract expiry itself&lt;/li&gt;&lt;li&gt;Overlooking a green patch with a great location &lt;/li&gt;&lt;li&gt;Huge Balconies&lt;/li&gt;&lt;li&gt;Generous Gardens&lt;/li&gt;&lt;li&gt;BBQ Area&lt;/li&gt;&lt;li&gt;Park &amp;amp; Kid&amp;#39;s Play Area&lt;/li&gt;&lt;li&gt;On the Park and Play Area&lt;/li&gt;&lt;li&gt;Large Plot &lt;/li&gt;&lt;li&gt;Golf Course Community&lt;/li&gt;&lt;li&gt;Perfect family living for any prospective Owners looking for a convenient location &lt;/li&gt;&lt;li&gt;Mall within walking distance&lt;/li&gt;&lt;li&gt;Well connected with the Shopping Mall, Restaurants, Education System and Sports.&lt;/li&gt;&lt;li&gt;Covered Parking&lt;/li&gt;&lt;/ul&gt;The exquisite villas at Sidra are designed exclusively for those with a taste for contemporary living. Everything you could need and want in the best of lifestyle living is within the community. This is where convenience meets you at the comfort of your home.&lt;br/&gt;&lt;br/&gt;For more information and viewing call our expert&lt;br/&gt;&lt;br/&gt;Mr. Amar Rupaney &lt;br/&gt;&lt;br/&gt;&lt;br/&gt;or visit www.gwp.ae for further details.</t>
+          <t>Golden Wave Properties Proudly Presents this amazing E5, 5-bedroom villa located in the heart of Dubai Hills Estate for Sale&lt;br /&gt;&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Spacious 5 bedroom Villa Type E5 for sale in Sidra&lt;/li&gt;&lt;li&gt;Large Corner Plot 6636 sqft in size&lt;/li&gt;&lt;li&gt;BUA 4109.00 SQ FT&lt;/li&gt;&lt;li&gt;Landscaped garden, Well Maintained&lt;/li&gt;&lt;li&gt;Rented for Dhs 560,000/- in ONE PAYMENT till February 2026 and notice has been served for the tenant to vacate at the time of contract expiry itself&lt;/li&gt;&lt;li&gt;Overlooking a green patch with a great location &lt;/li&gt;&lt;li&gt;Huge Balconies&lt;/li&gt;&lt;li&gt;Generous Gardens&lt;/li&gt;&lt;li&gt;BBQ Area&lt;/li&gt;&lt;li&gt;Park &amp;amp; Kid's Play Area&lt;/li&gt;&lt;li&gt;On the Park and Play Area&lt;/li&gt;&lt;li&gt;Large Plot &lt;/li&gt;&lt;li&gt;Golf Course Community&lt;/li&gt;&lt;li&gt;Perfect family living for any prospective Owners looking for a convenient location &lt;/li&gt;&lt;li&gt;Mall within walking distance&lt;/li&gt;&lt;li&gt;Well connected with the Shopping Mall, Restaurants, Education System and Sports.&lt;/li&gt;&lt;li&gt;Covered Parking&lt;/li&gt;&lt;/ul&gt;The exquisite villas at Sidra are designed exclusively for those with a taste for contemporary living. Everything you could need and want in the best of lifestyle living is within the community. This is where convenience meets you at the comfort of your home.&lt;br /&gt;&lt;br /&gt;For more information and viewing call our expert&lt;br /&gt;&lt;br /&gt;Mr. Amar Rupaney &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;or visit www.gwp.ae for further details.</t>
         </is>
       </c>
     </row>
@@ -4530,7 +4524,7 @@
         </is>
       </c>
       <c r="P40" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
@@ -4618,7 +4612,7 @@
         </is>
       </c>
       <c r="P41" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
@@ -4706,7 +4700,7 @@
         </is>
       </c>
       <c r="P42" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
@@ -4790,7 +4784,7 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
@@ -4878,7 +4872,7 @@
         </is>
       </c>
       <c r="P44" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
@@ -4976,7 +4970,7 @@
         </is>
       </c>
       <c r="P45" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
@@ -5086,7 +5080,7 @@
         </is>
       </c>
       <c r="P46" t="n">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
@@ -5185,7 +5179,7 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
@@ -5282,7 +5276,7 @@
         </is>
       </c>
       <c r="P48" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
@@ -5384,7 +5378,7 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
@@ -5486,7 +5480,7 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
@@ -5589,7 +5583,7 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
@@ -5688,7 +5682,7 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
@@ -5792,7 +5786,7 @@
         </is>
       </c>
       <c r="P53" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
@@ -5893,7 +5887,7 @@
         </is>
       </c>
       <c r="P54" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
@@ -5956,7 +5950,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -5989,7 +5983,7 @@
         </is>
       </c>
       <c r="P55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
@@ -6008,7 +6002,7 @@
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Livrichy Real Estate is delighted to present this elegant villa for sale located in the highly sought-after Sidra 2 community within Dubai Hills Estate.&lt;/p&gt;&lt;br&gt;&lt;p&gt;Property Details:&lt;br/&gt;&lt;br/&gt;- Premium finishing&lt;br/&gt;- Full renovated (inside &amp;amp; out)&lt;br/&gt;- Private pool&lt;br/&gt;- BBQ and dining area, bar&lt;br/&gt;- Fully extended&lt;br/&gt;- Prime location&lt;br/&gt;- Large 4 bedroom &lt;br/&gt;- BUA: 4,640.86 sq ft&lt;br/&gt;&lt;br/&gt;This luxurious villa boasts a stunning infinity-edge pool, paired with a cozy fire pit lounge and a high-end outdoor culinary area - ideal for elegant gatherings and alfresco dining.&lt;br/&gt;&lt;/p&gt;&lt;br&gt;&lt;p&gt;Community Highlights:&lt;br/&gt;&lt;br/&gt;Family-friendly, secure environment&lt;br/&gt;Developed by Emaar in partnership with Meraas&lt;br/&gt;Located within Dubai’s premier golf course community&lt;br/&gt;18-hole championship golf course just minutes away&lt;br/&gt;Dubai Hills Mall nearby for retail, dining, and entertainment&lt;br/&gt;Two world-class hospitals, including King&amp;#39;s College London Hospital&lt;br/&gt;Quick access to top international schools: Brighton College, GEMS, Kings School (approx. 15 minutes)&lt;br/&gt;Seamless connectivity to Al Khail Road and Umm Suqeim Street&lt;/p&gt;&lt;br&gt;</t>
+          <t>&lt;p&gt;Livrichy Real Estate is delighted to present this elegant villa for sale located in the highly sought-after Sidra 2 community within Dubai Hills Estate.&lt;/p&gt;&lt;br /&gt;&lt;p&gt;Property Details:&lt;br /&gt;&lt;br /&gt;- Premium finishing&lt;br /&gt;- Full renovated (inside &amp;amp; out)&lt;br /&gt;- Private pool&lt;br /&gt;- BBQ and dining area, bar&lt;br /&gt;- Fully extended&lt;br /&gt;- Prime location&lt;br /&gt;- Large 4 bedroom &lt;br /&gt;- BUA: 4,640.86 sq ft&lt;br /&gt;&lt;br /&gt;This luxurious villa boasts a stunning infinity-edge pool, paired with a cozy fire pit lounge and a high-end outdoor culinary area - ideal for elegant gatherings and alfresco dining.&lt;br /&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;Community Highlights:&lt;br /&gt;&lt;br /&gt;Family-friendly, secure environment&lt;br /&gt;Developed by Emaar in partnership with Meraas&lt;br /&gt;Located within Dubai’s premier golf course community&lt;br /&gt;18-hole championship golf course just minutes away&lt;br /&gt;Dubai Hills Mall nearby for retail, dining, and entertainment&lt;br /&gt;Two world-class hospitals, including King's College London Hospital&lt;br /&gt;Quick access to top international schools: Brighton College, GEMS, Kings School (approx. 15 minutes)&lt;br /&gt;Seamless connectivity to Al Khail Road and Umm Suqeim Street&lt;/p&gt;&lt;br /&gt;</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6071,7 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
@@ -6161,7 +6155,7 @@
         </is>
       </c>
       <c r="P57" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
@@ -6227,7 +6221,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -6260,7 +6254,7 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
@@ -6361,7 +6355,7 @@
         </is>
       </c>
       <c r="P59" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
@@ -6463,7 +6457,7 @@
         </is>
       </c>
       <c r="P60" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
@@ -6563,7 +6557,7 @@
         </is>
       </c>
       <c r="P61" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
@@ -6670,7 +6664,7 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
@@ -6770,7 +6764,7 @@
         </is>
       </c>
       <c r="P63" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
@@ -6872,7 +6866,7 @@
         </is>
       </c>
       <c r="P64" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
@@ -6988,7 +6982,7 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
@@ -7097,7 +7091,7 @@
         </is>
       </c>
       <c r="P66" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
@@ -7200,7 +7194,7 @@
         </is>
       </c>
       <c r="P67" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
@@ -7306,7 +7300,7 @@
         </is>
       </c>
       <c r="P68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
@@ -7415,7 +7409,7 @@
         </is>
       </c>
       <c r="P69" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
@@ -7514,7 +7508,7 @@
         </is>
       </c>
       <c r="P70" t="n">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
@@ -7560,12 +7554,12 @@
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>RL457</t>
+          <t>SIDRA_III_V_S_MURAD</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-ii-14313865.html</t>
+          <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-iii-14537941.html</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -7580,7 +7574,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Sidra Villas II</t>
+          <t>Sidra Villas III</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -7589,10 +7583,10 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>15850000</v>
+        <v>7500000</v>
       </c>
       <c r="H71" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
@@ -7603,31 +7597,31 @@
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr">
         <is>
-          <t>6119</t>
+          <t>4420</t>
         </is>
       </c>
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr">
         <is>
-          <t>Luxury Furnished | Vibrant Community | Private Pool</t>
+          <t>With Maid Room | Standalone Villa | Exclusive Unit</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>2025-05-20</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="P71" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>Atif S. Jangda</t>
+          <t>Murad Raief Jened</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>WOW PROPERTIES</t>
+          <t>Real Estate Masters</t>
         </is>
       </c>
       <c r="S71" t="inlineStr">
@@ -7636,102 +7630,6 @@
         </is>
       </c>
       <c r="T71" t="inlineStr">
-        <is>
-          <t>WOW Properties is proud to present this luxury villa in Sidra Villas II, Dubai Hills Estates
-Property Details:
-- 5 Bedrooms Villa
-- BUA : 6,119.61sqft
-- Fully Furnished
-- Private Pool
-- Vacant on Transfer
-- Outdoor Pergola
-This villa is nestled in a prime, private location just moments from Dubai Hills Mall. Set on a generous plot, it offers exceptional space and overlooks the serene green belt. The garden features a charming pergola, and the property presents a fantastic renovation opportunity to create your dream home.
-Sidra is Dubai’s most vibrant and premium new community. Dubai Hills is strategically positioned on Al Khail Road and southeast of Downtown Dubai. The destination has an endless supply of nature trails and green spaces so you can live life in harmony with nature and world-class residential, hospitality and retail districts. The exquisite villas at Sidra are designed exclusively for those with a taste for contemporary living. The community is master-planned to connect you with some of the best choices in education, shopping, healthcare and sports.
-Dubai Hills Estate is a fully integrated community with luscious landscaped greens and pristine fairways with an iconic backdrop of the Burj Khalifa and the Dubai skyline.
-WOW Properties is a full service luxury real estate brokerage serving the Dubai market since 2019. Our team provides comprehensive services for buying, selling, leasing, and private development opportunities. We specialize in advisory services to help empower and educate our clients so they can make informed decisions and reach their real estate goals.
-For more information, please do not hesitate to contact us</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>SIDRA_III_V_S_MURAD</t>
-        </is>
-      </c>
-      <c r="B72" s="2" t="inlineStr">
-        <is>
-          <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-iii-14537941.html</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Dubai Hills Estate</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Sidra Villas</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Sidra Villas III</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G72" t="n">
-        <v>7500000</v>
-      </c>
-      <c r="H72" t="n">
-        <v>3</v>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr"/>
-      <c r="K72" t="inlineStr"/>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>4420</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr">
-        <is>
-          <t>With Maid Room | Standalone Villa | Exclusive Unit</t>
-        </is>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>2025-06-19</t>
-        </is>
-      </c>
-      <c r="P72" t="n">
-        <v>9</v>
-      </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>Murad Raief Jened</t>
-        </is>
-      </c>
-      <c r="R72" t="inlineStr">
-        <is>
-          <t>Real Estate Masters</t>
-        </is>
-      </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>Available</t>
-        </is>
-      </c>
-      <c r="T72" t="inlineStr">
         <is>
           <t xml:space="preserve">R E M Real Estate Brokers are pleased to bring to you:
 Sidra 3 – Dubai Hills Estate - Standalone Villa for Sale
@@ -7761,85 +7659,85 @@
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="1" t="inlineStr">
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
         <is>
           <t>SNNY-Sidra4BR</t>
         </is>
       </c>
-      <c r="B73" s="2" t="inlineStr">
+      <c r="B72" s="2" t="inlineStr">
         <is>
           <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-i-14198886.html</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>Dubai Hills Estate</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>Sidra Villas</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>Sidra Villas I</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="F72" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G73" t="n">
+      <c r="G72" t="n">
         <v>10200000</v>
       </c>
-      <c r="H73" t="n">
+      <c r="H72" t="n">
         <v>4</v>
       </c>
-      <c r="I73" t="inlineStr">
+      <c r="I72" t="inlineStr">
         <is>
           <t>Villa</t>
         </is>
       </c>
-      <c r="J73" t="inlineStr"/>
-      <c r="K73" t="inlineStr"/>
-      <c r="L73" t="inlineStr">
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr">
         <is>
           <t>3523</t>
         </is>
       </c>
-      <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr">
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr">
         <is>
           <t>Vacant / No Upgrades / Single Row / Furnished / E3</t>
         </is>
       </c>
-      <c r="O73" t="inlineStr">
+      <c r="O72" t="inlineStr">
         <is>
           <t>2025-05-07</t>
         </is>
       </c>
-      <c r="P73" t="n">
-        <v>52</v>
-      </c>
-      <c r="Q73" t="inlineStr">
+      <c r="P72" t="n">
+        <v>54</v>
+      </c>
+      <c r="Q72" t="inlineStr">
         <is>
           <t>Sunny Adhiya</t>
         </is>
       </c>
-      <c r="R73" t="inlineStr">
+      <c r="R72" t="inlineStr">
         <is>
           <t>Dynasty Real Estate - Head Office</t>
         </is>
       </c>
-      <c r="S73" t="inlineStr">
+      <c r="S72" t="inlineStr">
         <is>
           <t>Available</t>
         </is>
       </c>
-      <c r="T73" t="inlineStr">
+      <c r="T72" t="inlineStr">
         <is>
           <t xml:space="preserve">II No Agents II
 II 1 Day Prior Notice required II
@@ -7870,85 +7768,85 @@
         </is>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="1" t="inlineStr">
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
         <is>
           <t>SNNY-Sidra5Bed</t>
         </is>
       </c>
-      <c r="B74" s="2" t="inlineStr">
+      <c r="B73" s="2" t="inlineStr">
         <is>
           <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-ii-14200661.html</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>Dubai Hills Estate</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>Sidra Villas</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>Sidra Villas II</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr">
+      <c r="F73" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G74" t="n">
+      <c r="G73" t="n">
         <v>14500000</v>
       </c>
-      <c r="H74" t="n">
+      <c r="H73" t="n">
         <v>5</v>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="I73" t="inlineStr">
         <is>
           <t>Villa</t>
         </is>
       </c>
-      <c r="J74" t="inlineStr"/>
-      <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr">
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr">
         <is>
           <t>4283</t>
         </is>
       </c>
-      <c r="M74" t="inlineStr"/>
-      <c r="N74" t="inlineStr">
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr">
         <is>
           <t>Vacant Soon / Single Row / E5 / No Upgrades / 5BR</t>
         </is>
       </c>
-      <c r="O74" t="inlineStr">
+      <c r="O73" t="inlineStr">
         <is>
           <t>2025-05-07</t>
         </is>
       </c>
-      <c r="P74" t="n">
-        <v>52</v>
-      </c>
-      <c r="Q74" t="inlineStr">
+      <c r="P73" t="n">
+        <v>54</v>
+      </c>
+      <c r="Q73" t="inlineStr">
         <is>
           <t>Sunny Adhiya</t>
         </is>
       </c>
-      <c r="R74" t="inlineStr">
+      <c r="R73" t="inlineStr">
         <is>
           <t>Dynasty Real Estate - Head Office</t>
         </is>
       </c>
-      <c r="S74" t="inlineStr">
+      <c r="S73" t="inlineStr">
         <is>
           <t>Available</t>
         </is>
       </c>
-      <c r="T74" t="inlineStr">
+      <c r="T73" t="inlineStr">
         <is>
           <t>II No Agents II
 II 1 Day Prior Notice required II
@@ -7978,6 +7876,115 @@
         </is>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>SP-S-5867</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-iii-14468995.html</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Dubai Hills Estate</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Sidra Villas</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Sidra Villas III</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>11999999</v>
+      </c>
+      <c r="H74" t="n">
+        <v>4</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Villa</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>4901</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>4901</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>Furnished | Near to Park | Single Row | Type E3</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>2025-06-11</t>
+        </is>
+      </c>
+      <c r="P74" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>Ali Zafar</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>Springfield Real Estate</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>Spring Field Real Estate offers you Fully Furnished 4 Bedroom Villa for sale located in Sidra Villas 3.
+Property Features:
+	•	4 Bedrooms + Maids Room
+	•	4 Bathrooms
+	•	Type E3 Layout
+	•	Plot Size: 4,901.67 sq.ft
+	•	Modern open-plan kitchen
+	•	Floor-to-ceiling windows for natural light
+	•	Landscaped garden
+	•	Covered parking for 2 cars
+Community Highlights:
+	•	Gated community with 24/7 security
+	•	Walking distance to Dubai Hills Park
+	•	Minutes from Dubai Hills Mall
+	•	Access to top-rated schools and healthcare facilities
+	•	Community pool, gym, and kids’ play areas
+About the Community:
+Experience luxury living in the heart of Dubai Hills Estate with this beautifully maintained 4-bedroom Sidra Villa in the highly sought-after Sidra 3 community. Offering a perfect blend of modern architecture and family-friendly design, this home is ideal for those who value space, comfort, and location. This villa is perfect for families looking for a serene yet connected lifestyle, with easy access to Al Khail Road and Downtown Dubai.
+Springfield Real Estate provides a diverse range of properties for both sale and rent from Apartments, Villas, Townhouses and Plots.
+For more information, you may contact our specialist ( Ali Zafar) for more information.
+SPRING FIELD REAL ESTATE
+RERA ORN: 11929</t>
+        </is>
+      </c>
+    </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
         <is>
@@ -8043,7 +8050,7 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
@@ -8131,7 +8138,7 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
@@ -8226,7 +8233,7 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
@@ -8340,7 +8347,7 @@
         </is>
       </c>
       <c r="P78" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q78" t="inlineStr">
         <is>
@@ -8448,7 +8455,7 @@
         </is>
       </c>
       <c r="P79" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
@@ -8564,7 +8571,7 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
@@ -8677,7 +8684,7 @@
         </is>
       </c>
       <c r="P81" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
@@ -8778,7 +8785,7 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
@@ -8877,7 +8884,7 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
@@ -8964,7 +8971,7 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
@@ -9062,7 +9069,7 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
@@ -9164,7 +9171,7 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
@@ -9264,7 +9271,7 @@
         </is>
       </c>
       <c r="P87" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
@@ -9365,7 +9372,7 @@
         </is>
       </c>
       <c r="P88" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
@@ -9464,7 +9471,7 @@
         </is>
       </c>
       <c r="P89" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Q89" t="inlineStr">
         <is>
@@ -9561,7 +9568,7 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
@@ -9628,7 +9635,7 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>10500000</v>
+        <v>9500000</v>
       </c>
       <c r="H91" t="n">
         <v>4</v>
@@ -9657,7 +9664,7 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
@@ -9756,7 +9763,7 @@
         </is>
       </c>
       <c r="P92" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
@@ -9854,7 +9861,7 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
@@ -9948,7 +9955,7 @@
         </is>
       </c>
       <c r="P94" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
@@ -10046,7 +10053,7 @@
         </is>
       </c>
       <c r="P95" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q95" t="inlineStr">
         <is>
@@ -10146,7 +10153,7 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -10247,7 +10254,7 @@
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -10344,7 +10351,7 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
@@ -10442,7 +10449,7 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
@@ -10549,7 +10556,7 @@
         </is>
       </c>
       <c r="P100" t="n">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="Q100" t="inlineStr">
         <is>
@@ -10645,7 +10652,7 @@
         </is>
       </c>
       <c r="P101" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
@@ -10757,7 +10764,7 @@
         </is>
       </c>
       <c r="P102" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
@@ -10854,7 +10861,7 @@
         </is>
       </c>
       <c r="P103" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
@@ -10947,7 +10954,7 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
@@ -11058,7 +11065,7 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
@@ -11166,7 +11173,7 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
@@ -11278,7 +11285,7 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
@@ -11381,7 +11388,7 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
@@ -11503,7 +11510,7 @@
         </is>
       </c>
       <c r="P109" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
@@ -11615,7 +11622,7 @@
         </is>
       </c>
       <c r="P110" t="n">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
@@ -11734,7 +11741,7 @@
         </is>
       </c>
       <c r="P111" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
@@ -11832,7 +11839,7 @@
         </is>
       </c>
       <c r="P112" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q112" t="inlineStr">
         <is>
@@ -11881,12 +11888,12 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>SP-S-5867</t>
+          <t>LXF-S-71675</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
         <is>
-          <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-iii-14468995.html</t>
+          <t>https://www.propertyfinder.ae/en/plp/buy/villa-for-sale-dubai-dubai-hills-estate-sidra-villas-sidra-villas-iii-13798922.html</t>
         </is>
       </c>
       <c r="C113" s="4" t="inlineStr">
@@ -11910,7 +11917,7 @@
         </is>
       </c>
       <c r="G113" s="4" t="n">
-        <v>11999999</v>
+        <v>15500000</v>
       </c>
       <c r="H113" s="4" t="n">
         <v>4</v>
@@ -11924,35 +11931,31 @@
       <c r="K113" s="4" t="inlineStr"/>
       <c r="L113" s="5" t="inlineStr">
         <is>
-          <t>4901</t>
-        </is>
-      </c>
-      <c r="M113" s="6" t="inlineStr">
-        <is>
-          <t>4901</t>
-        </is>
-      </c>
+          <t>4926</t>
+        </is>
+      </c>
+      <c r="M113" s="4" t="inlineStr"/>
       <c r="N113" s="4" t="inlineStr">
         <is>
-          <t>Furnished | Near to Park | Single Row | Type E3</t>
+          <t>Fully Upgraded | Extended | Swimming Pool | Vacant</t>
         </is>
       </c>
       <c r="O113" s="4" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="P113" s="4" t="n">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="Q113" s="4" t="inlineStr">
         <is>
-          <t>Ali Zafar</t>
+          <t>Harrison Fry</t>
         </is>
       </c>
       <c r="R113" s="4" t="inlineStr">
         <is>
-          <t>Springfield Real Estate</t>
+          <t>Luxfolio Real Estate Brokers LLC</t>
         </is>
       </c>
       <c r="S113" s="4" t="inlineStr">
@@ -11962,28 +11965,12 @@
       </c>
       <c r="T113" s="4" t="inlineStr">
         <is>
-          <t>Spring Field Real Estate offers you Fully Furnished 4 Bedroom Villa for sale located in Sidra Villas 3.
-Property Features:
-	•	4 Bedrooms + Maids Room
-	•	4 Bathrooms
-	•	Type E3 Layout
-	•	Plot Size: 4,901.67 sq.ft
-	•	Modern open-plan kitchen
-	•	Floor-to-ceiling windows for natural light
-	•	Landscaped garden
-	•	Covered parking for 2 cars
-Community Highlights:
-	•	Gated community with 24/7 security
-	•	Walking distance to Dubai Hills Park
-	•	Minutes from Dubai Hills Mall
-	•	Access to top-rated schools and healthcare facilities
-	•	Community pool, gym, and kids’ play areas
-About the Community:
-Experience luxury living in the heart of Dubai Hills Estate with this beautifully maintained 4-bedroom Sidra Villa in the highly sought-after Sidra 3 community. Offering a perfect blend of modern architecture and family-friendly design, this home is ideal for those who value space, comfort, and location. This villa is perfect for families looking for a serene yet connected lifestyle, with easy access to Al Khail Road and Downtown Dubai.
-Springfield Real Estate provides a diverse range of properties for both sale and rent from Apartments, Villas, Townhouses and Plots.
-For more information, you may contact our specialist ( Ali Zafar) for more information.
-SPRING FIELD REAL ESTATE
-RERA ORN: 11929</t>
+          <t>Luxfolio are proud to sell this beautiful, fully upgraded and extended 4 bedroom villa in Sidra, Dubai Hills.
+Discover unparalleled luxury in this fully upgraded and extended 4-bedroom villa located in the prestigious Sidra community of Dubai Hills. 
+This exceptional home offers a perfect blend of modern elegance and comfort, featuring a spacious open-plan layout with high-end finishes throughout. The state-of-the-art kitchen is a chef&amp;#39;s dream, equipped with premium appliances and custom cabinetry.
+ The expansive living and dining areas are ideal for entertaining, with large windows providing abundant natural light and stunning views of the landscaped garden. Each of the four bedrooms is generously sized, with the master suite offering a private retreat complete with a luxurious en-suite bathroom and walk-in closet. 
+The villa has been thoughtfully extended to include additional living space, perfect for a home office or family room. Outside, the beautifully landscaped garden offers a serene oasis, ideal for outdoor gatherings or relaxation. 
+Residents of Sidra enjoy access to world-class amenities, including a community pool, fitness center, and parks. Situated in the heart of Dubai Hills, this villa offers convenient access to top schools, shopping centers, and major roadways. Experience the ultimate in luxury living in this stunning Sidra villa</t>
         </is>
       </c>
     </row>

</xml_diff>